<commit_message>
Removed 'Signature' feature from data and dictionary
</commit_message>
<xml_diff>
--- a/Data/packs.xlsx
+++ b/Data/packs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="11">
   <si>
     <t xml:space="preserve">pack_number</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">g_legendaries</t>
   </si>
   <si>
-    <t xml:space="preserve">signatures</t>
-  </si>
-  <si>
     <t xml:space="preserve">expansion</t>
   </si>
   <si>
@@ -65,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,11 +83,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +132,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,17 +153,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,9 +197,6 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -225,8 +214,8 @@
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>11</v>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,8 +228,8 @@
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -256,8 +245,8 @@
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>11</v>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,8 +259,8 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>11</v>
+      <c r="J5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,8 +273,8 @@
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>11</v>
+      <c r="J6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,8 +287,8 @@
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>11</v>
+      <c r="J7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,8 +301,8 @@
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>11</v>
+      <c r="J8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,8 +318,8 @@
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>11</v>
+      <c r="J9" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,8 +335,8 @@
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>11</v>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,8 +349,8 @@
       <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>11</v>
+      <c r="J11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,8 +363,8 @@
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>11</v>
+      <c r="J12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,8 +377,8 @@
       <c r="C13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>11</v>
+      <c r="J13" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,8 +391,8 @@
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>11</v>
+      <c r="J14" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,8 +405,8 @@
       <c r="C15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>11</v>
+      <c r="J15" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,8 +419,8 @@
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>11</v>
+      <c r="J16" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,8 +436,8 @@
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>11</v>
+      <c r="J17" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,8 +450,8 @@
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>11</v>
+      <c r="J18" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,8 +464,8 @@
       <c r="C19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>11</v>
+      <c r="J19" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,8 +481,8 @@
       <c r="D20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>11</v>
+      <c r="J20" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,8 +495,8 @@
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>11</v>
+      <c r="J21" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,8 +512,8 @@
       <c r="E22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>11</v>
+      <c r="J22" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,8 +526,8 @@
       <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>11</v>
+      <c r="J23" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,8 +543,8 @@
       <c r="D24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>11</v>
+      <c r="J24" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,8 +557,8 @@
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>11</v>
+      <c r="J25" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,8 +574,8 @@
       <c r="F26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>11</v>
+      <c r="J26" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,8 +588,8 @@
       <c r="C27" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>11</v>
+      <c r="J27" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,8 +602,8 @@
       <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>11</v>
+      <c r="J28" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,8 +616,8 @@
       <c r="C29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>11</v>
+      <c r="J29" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,8 +633,8 @@
       <c r="G30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>11</v>
+      <c r="J30" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,8 +647,8 @@
       <c r="C31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>11</v>
+      <c r="J31" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,8 +664,8 @@
       <c r="D32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>11</v>
+      <c r="J32" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,8 +678,8 @@
       <c r="C33" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>11</v>
+      <c r="J33" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,8 +692,8 @@
       <c r="C34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>11</v>
+      <c r="J34" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,8 +706,8 @@
       <c r="C35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>11</v>
+      <c r="J35" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,8 +720,8 @@
       <c r="C36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>11</v>
+      <c r="J36" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,8 +740,8 @@
       <c r="F37" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>11</v>
+      <c r="J37" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,8 +754,8 @@
       <c r="C38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>11</v>
+      <c r="J38" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,8 +768,8 @@
       <c r="C39" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>11</v>
+      <c r="J39" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,8 +782,8 @@
       <c r="C40" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>11</v>
+      <c r="J40" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,8 +799,8 @@
       <c r="D41" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>11</v>
+      <c r="J41" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,8 +816,8 @@
       <c r="F42" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>11</v>
+      <c r="J42" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,8 +830,8 @@
       <c r="C43" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>11</v>
+      <c r="J43" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,8 +844,8 @@
       <c r="C44" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>11</v>
+      <c r="J44" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,8 +858,8 @@
       <c r="C45" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>11</v>
+      <c r="J45" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,8 +872,8 @@
       <c r="D46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K46" s="1" t="s">
-        <v>11</v>
+      <c r="J46" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,8 +886,8 @@
       <c r="C47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>11</v>
+      <c r="J47" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,8 +900,8 @@
       <c r="C48" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>11</v>
+      <c r="J48" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,8 +917,8 @@
       <c r="F49" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>11</v>
+      <c r="J49" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,8 +931,8 @@
       <c r="C50" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>11</v>
+      <c r="J50" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,8 +948,8 @@
       <c r="D51" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>11</v>
+      <c r="J51" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,8 +965,8 @@
       <c r="E52" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>11</v>
+      <c r="J52" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,8 +979,8 @@
       <c r="C53" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>11</v>
+      <c r="J53" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,8 +993,8 @@
       <c r="C54" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>11</v>
+      <c r="J54" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,8 +1010,8 @@
       <c r="G55" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>11</v>
+      <c r="J55" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,8 +1024,8 @@
       <c r="C56" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>11</v>
+      <c r="J56" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,8 +1041,8 @@
       <c r="F57" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K57" s="1" t="s">
-        <v>11</v>
+      <c r="J57" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,8 +1055,8 @@
       <c r="C58" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K58" s="1" t="s">
-        <v>11</v>
+      <c r="J58" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,8 +1069,8 @@
       <c r="C59" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>11</v>
+      <c r="J59" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,8 +1086,8 @@
       <c r="D60" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K60" s="1" t="s">
-        <v>11</v>
+      <c r="J60" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,8 +1100,8 @@
       <c r="C61" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>11</v>
+      <c r="J61" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,8 +1114,8 @@
       <c r="C62" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K62" s="1" t="s">
-        <v>11</v>
+      <c r="J62" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,8 +1128,8 @@
       <c r="C63" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K63" s="1" t="s">
-        <v>11</v>
+      <c r="J63" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,8 +1145,8 @@
       <c r="F64" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K64" s="1" t="s">
-        <v>11</v>
+      <c r="J64" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,8 +1159,8 @@
       <c r="C65" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K65" s="1" t="s">
-        <v>11</v>
+      <c r="J65" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,8 +1173,8 @@
       <c r="C66" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K66" s="1" t="s">
-        <v>11</v>
+      <c r="J66" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,8 +1187,8 @@
       <c r="C67" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K67" s="1" t="s">
-        <v>11</v>
+      <c r="J67" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,8 +1201,8 @@
       <c r="C68" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K68" s="1" t="s">
-        <v>11</v>
+      <c r="J68" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,8 +1218,8 @@
       <c r="D69" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K69" s="1" t="s">
-        <v>11</v>
+      <c r="J69" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,8 +1232,8 @@
       <c r="C70" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K70" s="1" t="s">
-        <v>11</v>
+      <c r="J70" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,8 +1249,8 @@
       <c r="D71" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K71" s="1" t="s">
-        <v>11</v>
+      <c r="J71" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,8 +1263,8 @@
       <c r="C72" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K72" s="1" t="s">
-        <v>11</v>
+      <c r="J72" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,8 +1280,8 @@
       <c r="D73" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K73" s="1" t="s">
-        <v>11</v>
+      <c r="J73" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,8 +1294,8 @@
       <c r="C74" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K74" s="1" t="s">
-        <v>11</v>
+      <c r="J74" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,8 +1311,8 @@
       <c r="D75" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>11</v>
+      <c r="J75" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,8 +1325,8 @@
       <c r="C76" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K76" s="1" t="s">
-        <v>11</v>
+      <c r="J76" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,8 +1339,8 @@
       <c r="C77" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K77" s="1" t="s">
-        <v>11</v>
+      <c r="J77" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,8 +1353,8 @@
       <c r="C78" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K78" s="1" t="s">
-        <v>11</v>
+      <c r="J78" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,8 +1367,8 @@
       <c r="C79" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K79" s="1" t="s">
-        <v>11</v>
+      <c r="J79" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1392,8 +1381,8 @@
       <c r="C80" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K80" s="1" t="s">
-        <v>11</v>
+      <c r="J80" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,8 +1395,8 @@
       <c r="C81" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K81" s="1" t="s">
-        <v>11</v>
+      <c r="J81" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,8 +1415,8 @@
       <c r="G82" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K82" s="1" t="s">
-        <v>11</v>
+      <c r="J82" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,8 +1432,8 @@
       <c r="D83" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K83" s="1" t="s">
-        <v>11</v>
+      <c r="J83" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,8 +1446,8 @@
       <c r="C84" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K84" s="1" t="s">
-        <v>11</v>
+      <c r="J84" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,8 +1460,8 @@
       <c r="C85" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K85" s="1" t="s">
-        <v>11</v>
+      <c r="J85" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,8 +1474,8 @@
       <c r="C86" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K86" s="1" t="s">
-        <v>11</v>
+      <c r="J86" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1499,8 +1488,8 @@
       <c r="C87" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K87" s="1" t="s">
-        <v>11</v>
+      <c r="J87" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,8 +1505,8 @@
       <c r="D88" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K88" s="1" t="s">
-        <v>11</v>
+      <c r="J88" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,8 +1519,8 @@
       <c r="C89" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K89" s="1" t="s">
-        <v>11</v>
+      <c r="J89" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,8 +1536,8 @@
       <c r="F90" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K90" s="1" t="s">
-        <v>11</v>
+      <c r="J90" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,8 +1556,8 @@
       <c r="F91" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K91" s="1" t="s">
-        <v>11</v>
+      <c r="J91" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,8 +1570,8 @@
       <c r="C92" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K92" s="1" t="s">
-        <v>11</v>
+      <c r="J92" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,8 +1587,8 @@
       <c r="D93" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K93" s="1" t="s">
-        <v>11</v>
+      <c r="J93" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,8 +1601,8 @@
       <c r="C94" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K94" s="1" t="s">
-        <v>11</v>
+      <c r="J94" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,8 +1615,8 @@
       <c r="C95" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K95" s="1" t="s">
-        <v>11</v>
+      <c r="J95" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,8 +1629,8 @@
       <c r="C96" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K96" s="1" t="s">
-        <v>11</v>
+      <c r="J96" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,8 +1643,8 @@
       <c r="C97" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K97" s="1" t="s">
-        <v>11</v>
+      <c r="J97" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,8 +1657,8 @@
       <c r="C98" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="K98" s="1" t="s">
-        <v>11</v>
+      <c r="J98" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,8 +1674,8 @@
       <c r="G99" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K99" s="1" t="s">
-        <v>11</v>
+      <c r="J99" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,8 +1688,8 @@
       <c r="C100" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K100" s="1" t="s">
-        <v>11</v>
+      <c r="J100" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,8 +1702,8 @@
       <c r="C101" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K101" s="1" t="s">
-        <v>11</v>
+      <c r="J101" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>